<commit_message>
working with home paths
</commit_message>
<xml_diff>
--- a/clean_data/site_time_series.xlsx
+++ b/clean_data/site_time_series.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="62">
   <si>
     <t>FIPS</t>
   </si>
@@ -58,145 +58,148 @@
     <t>Manitowoc, Wisconsin, US</t>
   </si>
   <si>
-    <t>3/19/20</t>
-  </si>
-  <si>
-    <t>3/20/20</t>
-  </si>
-  <si>
-    <t>3/21/20</t>
-  </si>
-  <si>
-    <t>3/22/20</t>
-  </si>
-  <si>
-    <t>3/23/20</t>
-  </si>
-  <si>
-    <t>3/24/20</t>
-  </si>
-  <si>
-    <t>3/25/20</t>
-  </si>
-  <si>
-    <t>3/26/20</t>
-  </si>
-  <si>
-    <t>3/27/20</t>
-  </si>
-  <si>
-    <t>3/28/20</t>
-  </si>
-  <si>
-    <t>3/29/20</t>
-  </si>
-  <si>
-    <t>3/30/20</t>
-  </si>
-  <si>
-    <t>3/31/20</t>
-  </si>
-  <si>
-    <t>4/1/20</t>
-  </si>
-  <si>
-    <t>4/2/20</t>
-  </si>
-  <si>
-    <t>4/3/20</t>
-  </si>
-  <si>
-    <t>4/4/20</t>
-  </si>
-  <si>
-    <t>4/5/20</t>
-  </si>
-  <si>
-    <t>4/6/20</t>
-  </si>
-  <si>
-    <t>4/7/20</t>
-  </si>
-  <si>
-    <t>4/8/20</t>
-  </si>
-  <si>
-    <t>4/9/20</t>
-  </si>
-  <si>
-    <t>4/10/20</t>
-  </si>
-  <si>
-    <t>4/11/20</t>
-  </si>
-  <si>
-    <t>4/12/20</t>
-  </si>
-  <si>
-    <t>4/13/20</t>
-  </si>
-  <si>
-    <t>4/14/20</t>
-  </si>
-  <si>
-    <t>4/15/20</t>
-  </si>
-  <si>
-    <t>4/16/20</t>
-  </si>
-  <si>
-    <t>4/17/20</t>
-  </si>
-  <si>
-    <t>4/18/20</t>
-  </si>
-  <si>
-    <t>4/19/20</t>
-  </si>
-  <si>
-    <t>4/20/20</t>
-  </si>
-  <si>
-    <t>4/21/20</t>
-  </si>
-  <si>
-    <t>4/22/20</t>
-  </si>
-  <si>
-    <t>4/23/20</t>
-  </si>
-  <si>
-    <t>4/24/20</t>
-  </si>
-  <si>
-    <t>4/25/20</t>
-  </si>
-  <si>
-    <t>4/26/20</t>
-  </si>
-  <si>
-    <t>4/27/20</t>
-  </si>
-  <si>
-    <t>4/28/20</t>
-  </si>
-  <si>
-    <t>4/29/20</t>
-  </si>
-  <si>
-    <t>4/30/20</t>
-  </si>
-  <si>
-    <t>5/1/20</t>
-  </si>
-  <si>
-    <t>5/2/20</t>
-  </si>
-  <si>
-    <t>5/3/20</t>
-  </si>
-  <si>
-    <t>5/4/20</t>
+    <t>2020-03-19</t>
+  </si>
+  <si>
+    <t>2020-03-20</t>
+  </si>
+  <si>
+    <t>2020-03-21</t>
+  </si>
+  <si>
+    <t>2020-03-22</t>
+  </si>
+  <si>
+    <t>2020-03-23</t>
+  </si>
+  <si>
+    <t>2020-03-24</t>
+  </si>
+  <si>
+    <t>2020-03-25</t>
+  </si>
+  <si>
+    <t>2020-03-26</t>
+  </si>
+  <si>
+    <t>2020-03-27</t>
+  </si>
+  <si>
+    <t>2020-03-28</t>
+  </si>
+  <si>
+    <t>2020-03-29</t>
+  </si>
+  <si>
+    <t>2020-03-30</t>
+  </si>
+  <si>
+    <t>2020-03-31</t>
+  </si>
+  <si>
+    <t>2020-04-01</t>
+  </si>
+  <si>
+    <t>2020-04-02</t>
+  </si>
+  <si>
+    <t>2020-04-03</t>
+  </si>
+  <si>
+    <t>2020-04-04</t>
+  </si>
+  <si>
+    <t>2020-04-05</t>
+  </si>
+  <si>
+    <t>2020-04-06</t>
+  </si>
+  <si>
+    <t>2020-04-07</t>
+  </si>
+  <si>
+    <t>2020-04-08</t>
+  </si>
+  <si>
+    <t>2020-04-09</t>
+  </si>
+  <si>
+    <t>2020-04-10</t>
+  </si>
+  <si>
+    <t>2020-04-11</t>
+  </si>
+  <si>
+    <t>2020-04-12</t>
+  </si>
+  <si>
+    <t>2020-04-13</t>
+  </si>
+  <si>
+    <t>2020-04-14</t>
+  </si>
+  <si>
+    <t>2020-04-15</t>
+  </si>
+  <si>
+    <t>2020-04-16</t>
+  </si>
+  <si>
+    <t>2020-04-17</t>
+  </si>
+  <si>
+    <t>2020-04-18</t>
+  </si>
+  <si>
+    <t>2020-04-19</t>
+  </si>
+  <si>
+    <t>2020-04-20</t>
+  </si>
+  <si>
+    <t>2020-04-21</t>
+  </si>
+  <si>
+    <t>2020-04-22</t>
+  </si>
+  <si>
+    <t>2020-04-23</t>
+  </si>
+  <si>
+    <t>2020-04-24</t>
+  </si>
+  <si>
+    <t>2020-04-25</t>
+  </si>
+  <si>
+    <t>2020-04-26</t>
+  </si>
+  <si>
+    <t>2020-04-27</t>
+  </si>
+  <si>
+    <t>2020-04-28</t>
+  </si>
+  <si>
+    <t>2020-04-29</t>
+  </si>
+  <si>
+    <t>2020-04-30</t>
+  </si>
+  <si>
+    <t>2020-05-01</t>
+  </si>
+  <si>
+    <t>2020-05-02</t>
+  </si>
+  <si>
+    <t>2020-05-03</t>
+  </si>
+  <si>
+    <t>2020-05-04</t>
+  </si>
+  <si>
+    <t>2020-05-05</t>
   </si>
 </sst>
 </file>
@@ -554,7 +557,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -646,7 +649,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>55061</v>
@@ -675,7 +678,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>55071</v>
@@ -704,7 +707,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>55061</v>
@@ -733,7 +736,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>55071</v>
@@ -762,7 +765,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>55061</v>
@@ -791,7 +794,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>55071</v>
@@ -820,7 +823,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>55061</v>
@@ -849,7 +852,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>55071</v>
@@ -878,7 +881,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>55061</v>
@@ -907,7 +910,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>55071</v>
@@ -936,7 +939,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>55061</v>
@@ -965,7 +968,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>55071</v>
@@ -994,7 +997,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>55061</v>
@@ -1023,7 +1026,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>55071</v>
@@ -1052,7 +1055,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>55061</v>
@@ -1081,7 +1084,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>55071</v>
@@ -1110,7 +1113,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="1">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>55061</v>
@@ -1139,7 +1142,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>55071</v>
@@ -1168,7 +1171,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>55061</v>
@@ -1197,7 +1200,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>55071</v>
@@ -1226,7 +1229,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>55061</v>
@@ -1255,7 +1258,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>55071</v>
@@ -1284,7 +1287,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>55061</v>
@@ -1313,7 +1316,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>55071</v>
@@ -1342,7 +1345,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>55061</v>
@@ -1371,7 +1374,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>55071</v>
@@ -1400,7 +1403,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="1">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>55061</v>
@@ -1429,7 +1432,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>55071</v>
@@ -1458,7 +1461,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>55061</v>
@@ -1487,7 +1490,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>55071</v>
@@ -1516,7 +1519,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <v>55061</v>
@@ -1545,7 +1548,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="1">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>55071</v>
@@ -1574,7 +1577,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="1">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <v>55061</v>
@@ -1603,7 +1606,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="1">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>55071</v>
@@ -1632,7 +1635,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>55061</v>
@@ -1661,7 +1664,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="1">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <v>55071</v>
@@ -1690,7 +1693,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="1">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>55061</v>
@@ -1719,7 +1722,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="1">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="B41">
         <v>55071</v>
@@ -1748,7 +1751,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="1">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B42">
         <v>55061</v>
@@ -1777,7 +1780,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="1">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="B43">
         <v>55071</v>
@@ -1806,7 +1809,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="1">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B44">
         <v>55061</v>
@@ -1835,7 +1838,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="B45">
         <v>55071</v>
@@ -1864,7 +1867,7 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="1">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="B46">
         <v>55061</v>
@@ -1893,7 +1896,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="1">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="B47">
         <v>55071</v>
@@ -1922,7 +1925,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="1">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="B48">
         <v>55061</v>
@@ -1951,7 +1954,7 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="1">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="B49">
         <v>55071</v>
@@ -1980,7 +1983,7 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="1">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="B50">
         <v>55061</v>
@@ -2009,7 +2012,7 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="1">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="B51">
         <v>55071</v>
@@ -2038,7 +2041,7 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="1">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="B52">
         <v>55061</v>
@@ -2067,7 +2070,7 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="1">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="B53">
         <v>55071</v>
@@ -2096,7 +2099,7 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="1">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="B54">
         <v>55061</v>
@@ -2125,7 +2128,7 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="1">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="B55">
         <v>55071</v>
@@ -2154,7 +2157,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="1">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="B56">
         <v>55061</v>
@@ -2183,7 +2186,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B57">
         <v>55071</v>
@@ -2212,7 +2215,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="1">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="B58">
         <v>55061</v>
@@ -2241,7 +2244,7 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="1">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="B59">
         <v>55071</v>
@@ -2270,7 +2273,7 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="1">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="B60">
         <v>55061</v>
@@ -2299,7 +2302,7 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="1">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="B61">
         <v>55071</v>
@@ -2328,7 +2331,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="1">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B62">
         <v>55061</v>
@@ -2357,7 +2360,7 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="1">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="B63">
         <v>55071</v>
@@ -2386,7 +2389,7 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="1">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="B64">
         <v>55061</v>
@@ -2415,7 +2418,7 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="1">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="B65">
         <v>55071</v>
@@ -2444,7 +2447,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="1">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="B66">
         <v>55061</v>
@@ -2473,7 +2476,7 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="1">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="B67">
         <v>55071</v>
@@ -2502,7 +2505,7 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="1">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="B68">
         <v>55061</v>
@@ -2531,7 +2534,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="1">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="B69">
         <v>55071</v>
@@ -2560,7 +2563,7 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="1">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="B70">
         <v>55061</v>
@@ -2589,7 +2592,7 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="1">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="B71">
         <v>55071</v>
@@ -2618,7 +2621,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="1">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="B72">
         <v>55061</v>
@@ -2647,7 +2650,7 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="1">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="B73">
         <v>55071</v>
@@ -2676,7 +2679,7 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="1">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="B74">
         <v>55061</v>
@@ -2705,7 +2708,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="1">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="B75">
         <v>55071</v>
@@ -2734,7 +2737,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="1">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="B76">
         <v>55061</v>
@@ -2763,7 +2766,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="1">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="B77">
         <v>55071</v>
@@ -2792,7 +2795,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="1">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="B78">
         <v>55061</v>
@@ -2821,7 +2824,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="1">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="B79">
         <v>55071</v>
@@ -2850,7 +2853,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="1">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="B80">
         <v>55061</v>
@@ -2879,7 +2882,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="1">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="B81">
         <v>55071</v>
@@ -2908,7 +2911,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="1">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="B82">
         <v>55061</v>
@@ -2937,7 +2940,7 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" s="1">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="B83">
         <v>55071</v>
@@ -2966,7 +2969,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="1">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="B84">
         <v>55061</v>
@@ -2995,7 +2998,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="1">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="B85">
         <v>55071</v>
@@ -3024,7 +3027,7 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" s="1">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="B86">
         <v>55061</v>
@@ -3053,7 +3056,7 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="1">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="B87">
         <v>55071</v>
@@ -3082,7 +3085,7 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="1">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="B88">
         <v>55061</v>
@@ -3111,7 +3114,7 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" s="1">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="B89">
         <v>55071</v>
@@ -3140,7 +3143,7 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="1">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="B90">
         <v>55061</v>
@@ -3169,7 +3172,7 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" s="1">
-        <v>1</v>
+        <v>89</v>
       </c>
       <c r="B91">
         <v>55071</v>
@@ -3198,7 +3201,7 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="B92">
         <v>55061</v>
@@ -3227,7 +3230,7 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" s="1">
-        <v>1</v>
+        <v>91</v>
       </c>
       <c r="B93">
         <v>55071</v>
@@ -3256,7 +3259,7 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" s="1">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="B94">
         <v>55061</v>
@@ -3285,7 +3288,7 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" s="1">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="B95">
         <v>55071</v>
@@ -3310,6 +3313,64 @@
       </c>
       <c r="I95" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>55061</v>
+      </c>
+      <c r="C96" t="s">
+        <v>8</v>
+      </c>
+      <c r="D96">
+        <v>3</v>
+      </c>
+      <c r="E96" t="s">
+        <v>9</v>
+      </c>
+      <c r="F96" t="s">
+        <v>11</v>
+      </c>
+      <c r="G96" t="s">
+        <v>12</v>
+      </c>
+      <c r="H96">
+        <v>22</v>
+      </c>
+      <c r="I96" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>55071</v>
+      </c>
+      <c r="C97" t="s">
+        <v>8</v>
+      </c>
+      <c r="D97">
+        <v>3</v>
+      </c>
+      <c r="E97" t="s">
+        <v>10</v>
+      </c>
+      <c r="F97" t="s">
+        <v>11</v>
+      </c>
+      <c r="G97" t="s">
+        <v>13</v>
+      </c>
+      <c r="H97">
+        <v>16</v>
+      </c>
+      <c r="I97" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated with rolling average
</commit_message>
<xml_diff>
--- a/clean_data/site_time_series.xlsx
+++ b/clean_data/site_time_series.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="64">
   <si>
     <t>FIPS</t>
   </si>
@@ -58,6 +58,9 @@
     <t>Manitowoc, Wisconsin, US</t>
   </si>
   <si>
+    <t>2020-03-18</t>
+  </si>
+  <si>
     <t>2020-03-19</t>
   </si>
   <si>
@@ -202,7 +205,7 @@
     <t>2020-05-05</t>
   </si>
   <si>
-    <t>2020-05-06</t>
+    <t>2020-05-07</t>
   </si>
 </sst>
 </file>
@@ -560,7 +563,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I99"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1572,7 +1575,7 @@
         <v>13</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35" t="s">
         <v>30</v>
@@ -1630,7 +1633,7 @@
         <v>13</v>
       </c>
       <c r="H37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I37" t="s">
         <v>31</v>
@@ -1659,7 +1662,7 @@
         <v>12</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38" t="s">
         <v>32</v>
@@ -1862,7 +1865,7 @@
         <v>13</v>
       </c>
       <c r="H45">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I45" t="s">
         <v>35</v>
@@ -1920,7 +1923,7 @@
         <v>13</v>
       </c>
       <c r="H47">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I47" t="s">
         <v>36</v>
@@ -2007,7 +2010,7 @@
         <v>12</v>
       </c>
       <c r="H50">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I50" t="s">
         <v>38</v>
@@ -2065,7 +2068,7 @@
         <v>12</v>
       </c>
       <c r="H52">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I52" t="s">
         <v>39</v>
@@ -2152,7 +2155,7 @@
         <v>13</v>
       </c>
       <c r="H55">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I55" t="s">
         <v>40</v>
@@ -2181,7 +2184,7 @@
         <v>12</v>
       </c>
       <c r="H56">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I56" t="s">
         <v>41</v>
@@ -2239,7 +2242,7 @@
         <v>12</v>
       </c>
       <c r="H58">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I58" t="s">
         <v>42</v>
@@ -2268,7 +2271,7 @@
         <v>13</v>
       </c>
       <c r="H59">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I59" t="s">
         <v>42</v>
@@ -2297,7 +2300,7 @@
         <v>12</v>
       </c>
       <c r="H60">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I60" t="s">
         <v>43</v>
@@ -2384,7 +2387,7 @@
         <v>13</v>
       </c>
       <c r="H63">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I63" t="s">
         <v>44</v>
@@ -2500,7 +2503,7 @@
         <v>13</v>
       </c>
       <c r="H67">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I67" t="s">
         <v>46</v>
@@ -2645,7 +2648,7 @@
         <v>12</v>
       </c>
       <c r="H72">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I72" t="s">
         <v>49</v>
@@ -2703,7 +2706,7 @@
         <v>12</v>
       </c>
       <c r="H74">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I74" t="s">
         <v>50</v>
@@ -2732,7 +2735,7 @@
         <v>13</v>
       </c>
       <c r="H75">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I75" t="s">
         <v>50</v>
@@ -2761,7 +2764,7 @@
         <v>12</v>
       </c>
       <c r="H76">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I76" t="s">
         <v>51</v>
@@ -2848,7 +2851,7 @@
         <v>13</v>
       </c>
       <c r="H79">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I79" t="s">
         <v>52</v>
@@ -2906,7 +2909,7 @@
         <v>13</v>
       </c>
       <c r="H81">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I81" t="s">
         <v>53</v>
@@ -2935,7 +2938,7 @@
         <v>12</v>
       </c>
       <c r="H82">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I82" t="s">
         <v>54</v>
@@ -2993,7 +2996,7 @@
         <v>12</v>
       </c>
       <c r="H84">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I84" t="s">
         <v>55</v>
@@ -3109,7 +3112,7 @@
         <v>12</v>
       </c>
       <c r="H88">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I88" t="s">
         <v>57</v>
@@ -3167,7 +3170,7 @@
         <v>12</v>
       </c>
       <c r="H90">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I90" t="s">
         <v>58</v>
@@ -3196,7 +3199,7 @@
         <v>13</v>
       </c>
       <c r="H91">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I91" t="s">
         <v>58</v>
@@ -3225,7 +3228,7 @@
         <v>12</v>
       </c>
       <c r="H92">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I92" t="s">
         <v>59</v>
@@ -3283,7 +3286,7 @@
         <v>12</v>
       </c>
       <c r="H94">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I94" t="s">
         <v>60</v>
@@ -3312,7 +3315,7 @@
         <v>13</v>
       </c>
       <c r="H95">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I95" t="s">
         <v>60</v>
@@ -3370,7 +3373,7 @@
         <v>13</v>
       </c>
       <c r="H97">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I97" t="s">
         <v>61</v>
@@ -3399,7 +3402,7 @@
         <v>12</v>
       </c>
       <c r="H98">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I98" t="s">
         <v>62</v>
@@ -3428,10 +3431,68 @@
         <v>13</v>
       </c>
       <c r="H99">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I99" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>55061</v>
+      </c>
+      <c r="C100" t="s">
+        <v>8</v>
+      </c>
+      <c r="D100">
+        <v>3</v>
+      </c>
+      <c r="E100" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G100" t="s">
+        <v>12</v>
+      </c>
+      <c r="H100">
+        <v>25</v>
+      </c>
+      <c r="I100" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>55071</v>
+      </c>
+      <c r="C101" t="s">
+        <v>8</v>
+      </c>
+      <c r="D101">
+        <v>3</v>
+      </c>
+      <c r="E101" t="s">
+        <v>10</v>
+      </c>
+      <c r="F101" t="s">
+        <v>11</v>
+      </c>
+      <c r="G101" t="s">
+        <v>13</v>
+      </c>
+      <c r="H101">
+        <v>17</v>
+      </c>
+      <c r="I101" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>